<commit_message>
labels updated __final v
</commit_message>
<xml_diff>
--- a/Models/Text Detector Model/samples test/AI-human dataset.xlsx
+++ b/Models/Text Detector Model/samples test/AI-human dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graduation-project\Models\Text Detector Model\samples test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CBFCAB-3DA9-4BDB-810A-1D84FD438450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE421015-52A8-4C5B-8C7E-A13C0E599B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,14 +566,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="121" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="160" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="59.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -789,10 +786,10 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -822,10 +819,10 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -844,10 +841,10 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -910,10 +907,10 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>